<commit_message>
Page Objects 99% complete
</commit_message>
<xml_diff>
--- a/DataProvider/inputData.xlsx
+++ b/DataProvider/inputData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
   <si>
     <t>Mervin</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>sadfgasdgsdgasdgsagsgdsgasg</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Test001_test</t>
+  </si>
+  <si>
+    <t>https://192.168.5.56:9443/ProcessPortal/jsp/index.jsp</t>
   </si>
 </sst>
 </file>
@@ -835,7 +844,7 @@
         <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +852,7 @@
         <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +876,7 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>